<commit_message>
not entirely sure what happened here?
</commit_message>
<xml_diff>
--- a/data/unclassified/Ratio Identifiers Update.xlsx
+++ b/data/unclassified/Ratio Identifiers Update.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chelsea\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaijagahm/Desktop/BluegillMorphologyDataDOC/data/unclassified/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A25D302C-66D8-4EBA-B0C9-98F4301AEC25}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18AB4729-CB04-F14F-93A8-5EFD1AF3B062}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7B0FAC57-BA79-4CA8-B4AD-B481D87B39B9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="14700" windowHeight="14020" xr2:uid="{7B0FAC57-BA79-4CA8-B4AD-B481D87B39B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -22,12 +22,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -42,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="25">
   <si>
     <t>PecFinLengths</t>
   </si>
@@ -115,6 +109,9 @@
   <si>
     <t>15.0-25.0</t>
   </si>
+  <si>
+    <t>KG</t>
+  </si>
 </sst>
 </file>
 
@@ -156,7 +153,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -178,29 +178,33 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="1" xr16:uid="{4AD9B50A-8D33-4085-A8EB-7E2C6C9098A4}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="7">
-    <queryTableFields count="6">
+  <queryTableRefresh nextId="8" unboundColumnsRight="1">
+    <queryTableFields count="7">
       <queryTableField id="1" name="PecFinLengths" tableColumnId="1"/>
       <queryTableField id="2" name="fishStdLength" tableColumnId="2"/>
       <queryTableField id="3" name="Ratio" tableColumnId="3"/>
       <queryTableField id="4" name="rangeDOC" tableColumnId="4"/>
       <queryTableField id="5" name="lakeDOC" tableColumnId="5"/>
       <queryTableField id="6" name="lakeID" tableColumnId="6"/>
+      <queryTableField id="7" dataBound="0" tableColumnId="7"/>
     </queryTableFields>
   </queryTableRefresh>
 </queryTable>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E7AEF24F-62FC-4023-8F0F-FD1EDA5E0211}" name="Ratio_Identifiers_Update" displayName="Ratio_Identifiers_Update" ref="A1:F219" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:F219" xr:uid="{D1AE168C-2614-4F80-9D99-B94765BD318B}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E7AEF24F-62FC-4023-8F0F-FD1EDA5E0211}" name="Ratio_Identifiers_Update" displayName="Ratio_Identifiers_Update" ref="A1:G219" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:G219" xr:uid="{D1AE168C-2614-4F80-9D99-B94765BD318B}"/>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{5FCF91A6-2012-4512-B143-456DBCE8A51F}" uniqueName="1" name="PecFinLengths" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{A63B8E22-4A66-4EA6-AEFC-5F7929BF9A44}" uniqueName="2" name="fishStdLength" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{D7DB9586-C8D8-4F73-95E2-9F2EDBDE7F01}" uniqueName="3" name="Ratio" queryTableFieldId="3"/>
-    <tableColumn id="4" xr3:uid="{150B4B83-9C8D-4763-90A6-E1317A7E003C}" uniqueName="4" name="rangeDOC" queryTableFieldId="4" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{150B4B83-9C8D-4763-90A6-E1317A7E003C}" uniqueName="4" name="rangeDOC" queryTableFieldId="4" dataDxfId="2"/>
     <tableColumn id="5" xr3:uid="{255871AB-E356-4F46-9A28-E1DE9BD4B1A9}" uniqueName="5" name="lakeDOC" queryTableFieldId="5"/>
-    <tableColumn id="6" xr3:uid="{23B30BF6-0249-433A-B9A7-F75391D44A1F}" uniqueName="6" name="lakeID" queryTableFieldId="6" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{23B30BF6-0249-433A-B9A7-F75391D44A1F}" uniqueName="6" name="lakeID" queryTableFieldId="6" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{85F291C2-A3CA-D846-9B95-25E47BF0CF15}" uniqueName="7" name="KG" queryTableFieldId="7" dataDxfId="0">
+      <calculatedColumnFormula>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -503,23 +507,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14789394-5A70-4F06-A0BE-2FBB30C937B9}">
-  <dimension ref="A1:F219"/>
+  <dimension ref="A1:G219"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A170" workbookViewId="0">
-      <selection activeCell="H177" sqref="H177"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -538,8 +542,11 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>39.217611230000003</v>
       </c>
@@ -558,8 +565,12 @@
       <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.24693390098445164</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>38.120775899999998</v>
       </c>
@@ -578,8 +589,12 @@
       <c r="F3" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.2483879874421942</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>32.052182479999999</v>
       </c>
@@ -598,8 +613,12 @@
       <c r="F4" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.2652767870957578</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>37.195801469999999</v>
       </c>
@@ -618,8 +637,12 @@
       <c r="F5" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.2644724225565655</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>39.765423849999998</v>
       </c>
@@ -638,8 +661,12 @@
       <c r="F6" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.27231154325319495</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>42.909360210000003</v>
       </c>
@@ -658,8 +685,12 @@
       <c r="F7" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.27507579034385832</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>37.72112783</v>
       </c>
@@ -678,8 +709,12 @@
       <c r="F8" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.29611766323158073</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>43.063613429999997</v>
       </c>
@@ -698,8 +733,12 @@
       <c r="F9" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.25794600091111869</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>39.165645949999998</v>
       </c>
@@ -718,8 +757,12 @@
       <c r="F10" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G10">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.26489960706523225</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>37.705191249999999</v>
       </c>
@@ -738,8 +781,12 @@
       <c r="F11" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G11">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.26909433144115097</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>40.786707970000002</v>
       </c>
@@ -758,8 +805,12 @@
       <c r="F12" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G12">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.27489222298654659</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>30.430909669999998</v>
       </c>
@@ -778,8 +829,12 @@
       <c r="F13" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G13">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.25955169818883106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>33.397675200000002</v>
       </c>
@@ -798,8 +853,12 @@
       <c r="F14" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G14">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.2686037610137631</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>24.650724610000001</v>
       </c>
@@ -818,8 +877,12 @@
       <c r="F15" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G15">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.29176344594383991</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>24.140118990000001</v>
       </c>
@@ -838,8 +901,12 @@
       <c r="F16" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G16">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.24379282525941842</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>22.283433819999999</v>
       </c>
@@ -858,8 +925,12 @@
       <c r="F17" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G17">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.24795882296773505</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>40.808418590000002</v>
       </c>
@@ -878,8 +949,12 @@
       <c r="F18" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G18">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.29219496072284284</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>33.337112580000003</v>
       </c>
@@ -898,8 +973,12 @@
       <c r="F19" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G19">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.2843203581545965</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>37.056820989999999</v>
       </c>
@@ -918,8 +997,12 @@
       <c r="F20" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G20">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.24794734387672374</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>33.589390109999997</v>
       </c>
@@ -938,8 +1021,12 @@
       <c r="F21" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G21">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.28117178400178533</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>37.743750820000002</v>
       </c>
@@ -958,8 +1045,12 @@
       <c r="F22" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G22">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.27565469461079661</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>32.240112250000003</v>
       </c>
@@ -978,8 +1069,12 @@
       <c r="F23" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G23">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.30858356718227986</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>25.061759129999999</v>
       </c>
@@ -998,8 +1093,12 @@
       <c r="F24" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G24">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.26499073444732457</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>31.06418266</v>
       </c>
@@ -1018,8 +1117,12 @@
       <c r="F25" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G25">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.29983942990257501</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>37.866541179999999</v>
       </c>
@@ -1038,8 +1141,12 @@
       <c r="F26" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G26">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.28374211731063781</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>34.098228720000002</v>
       </c>
@@ -1058,8 +1165,12 @@
       <c r="F27" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G27">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.28551001791187813</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>29.587289559999999</v>
       </c>
@@ -1078,8 +1189,12 @@
       <c r="F28" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G28">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.27253584622354382</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>32.833673099999999</v>
       </c>
@@ -1098,8 +1213,12 @@
       <c r="F29" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G29">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.2837253064312425</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>37.253276890000002</v>
       </c>
@@ -1118,8 +1237,12 @@
       <c r="F30" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G30">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.3000732512243231</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30.877858459999999</v>
       </c>
@@ -1138,8 +1261,12 @@
       <c r="F31" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G31">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.27450781289417259</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>41.610904759999997</v>
       </c>
@@ -1158,8 +1285,12 @@
       <c r="F32" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G32">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.29604763142168089</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>39.53833771</v>
       </c>
@@ -1178,8 +1309,12 @@
       <c r="F33" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G33">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.26148523068598378</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>34.863278559999998</v>
       </c>
@@ -1198,8 +1333,12 @@
       <c r="F34" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G34">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.27533982333667412</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>27.50806141</v>
       </c>
@@ -1218,8 +1357,12 @@
       <c r="F35" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G35">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.26398412153832534</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>29.13506173</v>
       </c>
@@ -1238,8 +1381,12 @@
       <c r="F36" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G36">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.26787187932231815</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>18.012433359999999</v>
       </c>
@@ -1258,8 +1405,12 @@
       <c r="F37" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G37">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.22342988891446564</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>28.944463590000002</v>
       </c>
@@ -1278,8 +1429,12 @@
       <c r="F38" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G38">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.24347390600953456</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>37.401426309999998</v>
       </c>
@@ -1298,8 +1453,12 @@
       <c r="F39" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G39">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.2738880402113002</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>31.783665490000001</v>
       </c>
@@ -1318,8 +1477,12 @@
       <c r="F40" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G40">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.26208661709177633</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>19.676202679999999</v>
       </c>
@@ -1338,8 +1501,12 @@
       <c r="F41" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G41">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.24063002136374753</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>32.820787469999999</v>
       </c>
@@ -1358,8 +1525,12 @@
       <c r="F42" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G42">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.28023908511453194</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>30.858687840000002</v>
       </c>
@@ -1378,8 +1549,12 @@
       <c r="F43" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G43">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.25976501092288451</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>29.77148725</v>
       </c>
@@ -1398,8 +1573,12 @@
       <c r="F44" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G44">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.26477362369308116</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>23.592855</v>
       </c>
@@ -1418,8 +1597,12 @@
       <c r="F45" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G45">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.19726926174290585</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>22.011744459999999</v>
       </c>
@@ -1438,8 +1621,12 @@
       <c r="F46" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G46">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.22568129404502074</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>35.37624667</v>
       </c>
@@ -1458,8 +1645,12 @@
       <c r="F47" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G47">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.33206672266930642</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>37.69160231</v>
       </c>
@@ -1478,8 +1669,12 @@
       <c r="F48" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G48">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.52676009648146482</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>24.271889829999999</v>
       </c>
@@ -1498,8 +1693,12 @@
       <c r="F49" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G49">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.22995932113699302</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>30.83625704</v>
       </c>
@@ -1518,8 +1717,12 @@
       <c r="F50" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G50">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.29780500045446368</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>29.40395608</v>
       </c>
@@ -1538,8 +1741,12 @@
       <c r="F51" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G51">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.42451612236628627</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>32.042448700000001</v>
       </c>
@@ -1558,8 +1765,12 @@
       <c r="F52" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G52">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.42500507386638742</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>33.74154214</v>
       </c>
@@ -1578,8 +1789,12 @@
       <c r="F53" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G53">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.43143470383604521</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>22.404088250000001</v>
       </c>
@@ -1598,8 +1813,12 @@
       <c r="F54" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G54">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.26648633239014408</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>21.856371920000001</v>
       </c>
@@ -1618,8 +1837,12 @@
       <c r="F55" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G55">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.25853231710309771</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>23.064808589999998</v>
       </c>
@@ -1638,8 +1861,12 @@
       <c r="F56" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G56">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.28775037652954499</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>25.153065739999999</v>
       </c>
@@ -1658,8 +1885,12 @@
       <c r="F57" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G57">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.44192263515566632</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>45.606163459999998</v>
       </c>
@@ -1678,8 +1909,12 @@
       <c r="F58" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G58">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.27323480437485609</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>46.473671099999997</v>
       </c>
@@ -1698,8 +1933,12 @@
       <c r="F59" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G59">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.29323439742291818</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>46.452522190000003</v>
       </c>
@@ -1718,8 +1957,12 @@
       <c r="F60" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G60">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.27413837741286018</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>46.207642049999997</v>
       </c>
@@ -1738,8 +1981,12 @@
       <c r="F61" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G61">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.31229875323563605</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>37.454167810000001</v>
       </c>
@@ -1758,8 +2005,12 @@
       <c r="F62" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G62">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.22159161989756893</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>43.719630389999999</v>
       </c>
@@ -1778,8 +2029,12 @@
       <c r="F63" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G63">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.33536958027149577</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>43.748223500000002</v>
       </c>
@@ -1798,8 +2053,12 @@
       <c r="F64" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G64">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.26966322599442677</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>41.33490346</v>
       </c>
@@ -1818,8 +2077,12 @@
       <c r="F65" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G65">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.2836829315843814</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>40.162445990000002</v>
       </c>
@@ -1838,8 +2101,12 @@
       <c r="F66" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G66">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.30395598897840365</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>43.402909719999997</v>
       </c>
@@ -1858,8 +2125,12 @@
       <c r="F67" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G67">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.26457415697191844</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>37.025942370000003</v>
       </c>
@@ -1878,8 +2149,12 @@
       <c r="F68" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G68">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.20252301188123725</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>37.925885379999997</v>
       </c>
@@ -1898,8 +2173,12 @@
       <c r="F69" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G69">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.24372010466765867</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>42.936400859999999</v>
       </c>
@@ -1918,8 +2197,12 @@
       <c r="F70" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G70">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.23695529049386135</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>41.18634995</v>
       </c>
@@ -1938,8 +2221,12 @@
       <c r="F71" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G71">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.29518309968026907</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>38.093246559999997</v>
       </c>
@@ -1958,8 +2245,12 @@
       <c r="F72" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G72">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.21969668442863038</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>40.621290520000002</v>
       </c>
@@ -1978,8 +2269,12 @@
       <c r="F73" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G73">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.25333468182264329</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>39.173568119999999</v>
       </c>
@@ -1998,8 +2293,12 @@
       <c r="F74" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G74">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.22121120378285966</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>39.597788600000001</v>
       </c>
@@ -2018,8 +2317,12 @@
       <c r="F75" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G75">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.25856857510132525</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>41.967021420000002</v>
       </c>
@@ -2038,8 +2341,12 @@
       <c r="F76" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G76">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.24392855623540782</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>40.125220329999998</v>
       </c>
@@ -2058,8 +2365,12 @@
       <c r="F77" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G77">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.2647474792795228</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>34.039600280000002</v>
       </c>
@@ -2078,8 +2389,12 @@
       <c r="F78" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G78">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.19823103200209652</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>38.412391470000003</v>
       </c>
@@ -2098,8 +2413,12 @@
       <c r="F79" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G79">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.24499172435547933</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>34.056756630000002</v>
       </c>
@@ -2118,8 +2437,12 @@
       <c r="F80" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G80">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.2110656610702111</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>36.796759559999998</v>
       </c>
@@ -2138,8 +2461,12 @@
       <c r="F81" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G81">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.23558369799992879</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>39.72966237</v>
       </c>
@@ -2158,8 +2485,12 @@
       <c r="F82" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G82">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.25472432605416534</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>32.984673319999999</v>
       </c>
@@ -2178,8 +2509,12 @@
       <c r="F83" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G83">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.24750870153465621</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>21.685255850000001</v>
       </c>
@@ -2198,8 +2533,12 @@
       <c r="F84" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G84">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.2680362722012587</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>28.954317540000002</v>
       </c>
@@ -2218,8 +2557,12 @@
       <c r="F85" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G85">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.28368483171299608</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>29.217702280000001</v>
       </c>
@@ -2238,8 +2581,12 @@
       <c r="F86" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G86">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.2899472921697504</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>36.594550730000002</v>
       </c>
@@ -2258,8 +2605,12 @@
       <c r="F87" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G87">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.31656458365089118</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>28.575668719999999</v>
       </c>
@@ -2278,8 +2629,12 @@
       <c r="F88" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G88">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.46944539671589924</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>29.929443150000001</v>
       </c>
@@ -2298,8 +2653,12 @@
       <c r="F89" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G89">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.32267636578410802</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>28.912904579999999</v>
       </c>
@@ -2318,8 +2677,12 @@
       <c r="F90" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G90">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.32362046502805203</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>32.15865342</v>
       </c>
@@ -2338,8 +2701,12 @@
       <c r="F91" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G91">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.48794205636998739</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>23.085475639999999</v>
       </c>
@@ -2358,8 +2725,12 @@
       <c r="F92" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G92">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.21354727764896869</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>28.262426510000001</v>
       </c>
@@ -2378,8 +2749,12 @@
       <c r="F93" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G93">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.28743025992058874</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>31.3580024</v>
       </c>
@@ -2398,8 +2773,12 @@
       <c r="F94" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G94">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.47565153761010492</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>28.69707184</v>
       </c>
@@ -2418,8 +2797,12 @@
       <c r="F95" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G95">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.27034865826825294</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>41.63673593</v>
       </c>
@@ -2438,8 +2821,12 @@
       <c r="F96" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G96">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.27596353841912336</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>39.467846739999999</v>
       </c>
@@ -2458,8 +2845,12 @@
       <c r="F97" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G97">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.30106260071568258</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>34.859109029999999</v>
       </c>
@@ -2478,8 +2869,12 @@
       <c r="F98" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G98">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.28993330381299925</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>37.84370388</v>
       </c>
@@ -2498,8 +2893,12 @@
       <c r="F99" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G99">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.27056893565978157</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>32.114490230000001</v>
       </c>
@@ -2518,8 +2917,12 @@
       <c r="F100" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G100">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.25462451973209888</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>33.385692130000002</v>
       </c>
@@ -2538,8 +2941,12 @@
       <c r="F101" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G101">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.26107993554251846</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>32.696414109999999</v>
       </c>
@@ -2558,8 +2965,12 @@
       <c r="F102" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G102">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.30721695706003033</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>40.092998029999997</v>
       </c>
@@ -2578,8 +2989,12 @@
       <c r="F103" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G103">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.28916023586521689</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>26.290990019999999</v>
       </c>
@@ -2598,8 +3013,12 @@
       <c r="F104" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G104">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.29183291700743208</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>35.418463969999998</v>
       </c>
@@ -2618,8 +3037,12 @@
       <c r="F105" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G105">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.27846328660535608</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>35.957480570000001</v>
       </c>
@@ -2638,8 +3061,12 @@
       <c r="F106" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G106">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.30186857094785535</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>33.72319229</v>
       </c>
@@ -2658,8 +3085,12 @@
       <c r="F107" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G107">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.28627170965777898</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>21.84433799</v>
       </c>
@@ -2678,8 +3109,12 @@
       <c r="F108" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G108">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.27065787311537959</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>26.356693270000001</v>
       </c>
@@ -2698,8 +3133,12 @@
       <c r="F109" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G109">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.37196445836982633</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>22.257815659999999</v>
       </c>
@@ -2718,8 +3157,12 @@
       <c r="F110" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G110">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.25078209152159087</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>28.612128519999999</v>
       </c>
@@ -2738,8 +3181,12 @@
       <c r="F111" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G111">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.33278633173016692</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>25.58450861</v>
       </c>
@@ -2758,8 +3205,12 @@
       <c r="F112" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G112">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.31840860430991319</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>20.873126030000002</v>
       </c>
@@ -2778,8 +3229,12 @@
       <c r="F113" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G113">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.25490178298056865</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>38.177885490000001</v>
       </c>
@@ -2798,8 +3253,12 @@
       <c r="F114" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G114">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.26282949685346857</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>40.62875468</v>
       </c>
@@ -2818,8 +3277,12 @@
       <c r="F115" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G115">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.25003335462874987</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>39.988456990000003</v>
       </c>
@@ -2838,8 +3301,12 @@
       <c r="F116" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G116">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.25911287849198661</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>36.872888869999997</v>
       </c>
@@ -2858,8 +3325,12 @@
       <c r="F117" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G117">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.24803221962840366</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>35.348782239999998</v>
       </c>
@@ -2878,8 +3349,12 @@
       <c r="F118" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G118">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.26485594862703721</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>42.416549359999998</v>
       </c>
@@ -2898,8 +3373,12 @@
       <c r="F119" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G119">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.28370121542424764</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>43.493112760000002</v>
       </c>
@@ -2918,8 +3397,12 @@
       <c r="F120" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G120">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.27018337734305969</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>39.253950160000002</v>
       </c>
@@ -2938,8 +3421,12 @@
       <c r="F121" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G121">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.27817672312714786</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>37.323122429999998</v>
       </c>
@@ -2958,8 +3445,12 @@
       <c r="F122" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G122">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.25850878697664886</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>35.83905627</v>
       </c>
@@ -2978,8 +3469,12 @@
       <c r="F123" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G123">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.26986086495928557</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>35.331452040000002</v>
       </c>
@@ -2998,8 +3493,12 @@
       <c r="F124" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G124">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.2670971416269331</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>33.167434800000002</v>
       </c>
@@ -3018,8 +3517,12 @@
       <c r="F125" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G125">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.26410046269966492</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>30.059542579999999</v>
       </c>
@@ -3038,8 +3541,12 @@
       <c r="F126" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G126">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.26333897313075477</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>38.947532000000002</v>
       </c>
@@ -3058,8 +3565,12 @@
       <c r="F127" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G127">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.26603748750675055</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>41.233907279999997</v>
       </c>
@@ -3078,8 +3589,12 @@
       <c r="F128" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G128">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.26718053273551662</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>32.297860720000003</v>
       </c>
@@ -3098,8 +3613,12 @@
       <c r="F129" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G129">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.23015487856842134</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>20.89752399</v>
       </c>
@@ -3118,8 +3637,12 @@
       <c r="F130" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G130">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.24764464896675273</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>36.614747520000002</v>
       </c>
@@ -3138,8 +3661,12 @@
       <c r="F131" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G131">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.3193978480953929</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>25.483106920000001</v>
       </c>
@@ -3158,8 +3685,12 @@
       <c r="F132" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G132">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.29631104473735381</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>32.305428020000001</v>
       </c>
@@ -3178,8 +3709,12 @@
       <c r="F133" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G133">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.28299717804962421</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>23.182805500000001</v>
       </c>
@@ -3198,8 +3733,12 @@
       <c r="F134" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G134">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.29921202346201886</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>32.392585339999997</v>
       </c>
@@ -3218,8 +3757,12 @@
       <c r="F135" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G135">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.27957964958068848</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>27.268881310000001</v>
       </c>
@@ -3238,8 +3781,12 @@
       <c r="F136" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G136">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.31291392831123205</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>29.381137299999999</v>
       </c>
@@ -3258,8 +3805,12 @@
       <c r="F137" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G137">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.30160969528838655</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>35.050285690000003</v>
       </c>
@@ -3278,8 +3829,12 @@
       <c r="F138" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G138">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.29140950536852206</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>26.548398649999999</v>
       </c>
@@ -3298,8 +3853,12 @@
       <c r="F139" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G139">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.28255807461846982</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>29.208384500000001</v>
       </c>
@@ -3318,8 +3877,12 @@
       <c r="F140" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G140">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.30967813605187833</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>34.9118396</v>
       </c>
@@ -3338,8 +3901,12 @@
       <c r="F141" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G141">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.29299569598070657</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>24.60514405</v>
       </c>
@@ -3358,8 +3925,12 @@
       <c r="F142" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G142">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.28653611477537633</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>35.129920970000001</v>
       </c>
@@ -3378,8 +3949,12 @@
       <c r="F143" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G143">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.30104670154500079</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>33.296736260000003</v>
       </c>
@@ -3398,8 +3973,12 @@
       <c r="F144" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G144">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.31592368721624037</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>41.155077509999998</v>
       </c>
@@ -3418,8 +3997,12 @@
       <c r="F145" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G145">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.31618800608688613</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>26.159150879999999</v>
       </c>
@@ -3438,8 +4021,12 @@
       <c r="F146" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G146">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.20407219690835252</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>33.212263210000003</v>
       </c>
@@ -3458,8 +4045,12 @@
       <c r="F147" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G147">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.29592003432645198</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>36.497725000000003</v>
       </c>
@@ -3478,8 +4069,12 @@
       <c r="F148" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G148">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.40502826549411108</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>33.700471120000003</v>
       </c>
@@ -3498,8 +4093,12 @@
       <c r="F149" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G149">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.33348902817881049</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>27.15659114</v>
       </c>
@@ -3518,8 +4117,12 @@
       <c r="F150" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G150">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.21887378806446428</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>41.28946663</v>
       </c>
@@ -3538,8 +4141,12 @@
       <c r="F151" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G151">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.35513506866393024</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>34.689562639999998</v>
       </c>
@@ -3558,8 +4165,12 @@
       <c r="F152" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G152">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.2647196586637115</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>27.456617120000001</v>
       </c>
@@ -3578,8 +4189,12 @@
       <c r="F153" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G153">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.33736836558952399</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>30.607594599999999</v>
       </c>
@@ -3598,8 +4213,12 @@
       <c r="F154" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G154">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.23815235698809004</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>29.46855643</v>
       </c>
@@ -3618,8 +4237,12 @@
       <c r="F155" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G155">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.23912722927785793</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>30.251609290000001</v>
       </c>
@@ -3638,8 +4261,12 @@
       <c r="F156" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G156">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.26447840739865924</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>33.470947369999998</v>
       </c>
@@ -3658,8 +4285,12 @@
       <c r="F157" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G157">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.34130221726271054</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>30.059542579999999</v>
       </c>
@@ -3678,8 +4309,12 @@
       <c r="F158" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G158">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.25727455322468507</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>28.111972260000002</v>
       </c>
@@ -3698,8 +4333,12 @@
       <c r="F159" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G159">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.2256336473998099</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>34.161712989999998</v>
       </c>
@@ -3718,8 +4357,12 @@
       <c r="F160" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G160">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.29325109813402528</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>32.308023069999997</v>
       </c>
@@ -3738,8 +4381,12 @@
       <c r="F161" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G161">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.20532686298270428</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>34.292282069999999</v>
       </c>
@@ -3758,8 +4405,12 @@
       <c r="F162" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G162">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.28648538469763835</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>24.8334817</v>
       </c>
@@ -3778,8 +4429,12 @@
       <c r="F163" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G163">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.2383987506684753</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>27.774184689999998</v>
       </c>
@@ -3798,8 +4453,12 @@
       <c r="F164" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G164">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.29195174690783521</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>25.74199578</v>
       </c>
@@ -3818,8 +4477,12 @@
       <c r="F165" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G165">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.30507345473795833</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>25.702142569999999</v>
       </c>
@@ -3838,8 +4501,12 @@
       <c r="F166" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G166">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.23897871705399307</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>34.58364237</v>
       </c>
@@ -3858,8 +4525,12 @@
       <c r="F167" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G167">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.32383385162751249</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>25.914138860000001</v>
       </c>
@@ -3878,8 +4549,12 @@
       <c r="F168" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G168">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.31031213938647412</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>28.15284239</v>
       </c>
@@ -3898,8 +4573,12 @@
       <c r="F169" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G169">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.22808803909267938</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>30.729828139999999</v>
       </c>
@@ -3918,8 +4597,12 @@
       <c r="F170" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G170">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.31088313360156017</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>28.213843610000001</v>
       </c>
@@ -3938,8 +4621,12 @@
       <c r="F171" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G171">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.32416622050794186</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>33.761752549999997</v>
       </c>
@@ -3958,8 +4645,12 @@
       <c r="F172" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G172">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.33218524014242246</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>28.72560842</v>
       </c>
@@ -3978,8 +4669,12 @@
       <c r="F173" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G173">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.34487601499351667</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>29.738719010000001</v>
       </c>
@@ -3998,8 +4693,12 @@
       <c r="F174" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G174">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.35400188058612886</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>27.022468020000002</v>
       </c>
@@ -4018,8 +4717,12 @@
       <c r="F175" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G175">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.27411652611282089</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>24.13978071</v>
       </c>
@@ -4038,8 +4741,12 @@
       <c r="F176" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G176">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.28785317691587942</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>37.991600030000001</v>
       </c>
@@ -4058,8 +4765,12 @@
       <c r="F177" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G177">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.26747886946784483</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>44.808176490000001</v>
       </c>
@@ -4078,8 +4789,12 @@
       <c r="F178" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G178">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.29776403475525232</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>41.631557899999997</v>
       </c>
@@ -4098,8 +4813,12 @@
       <c r="F179" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G179">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.30338111605803658</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>38.782523910000002</v>
       </c>
@@ -4118,8 +4837,12 @@
       <c r="F180" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G180">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.25879252774623701</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>40.214774779999999</v>
       </c>
@@ -4138,8 +4861,12 @@
       <c r="F181" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G181">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.26899084085839903</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>38.93167794</v>
       </c>
@@ -4158,8 +4885,12 @@
       <c r="F182" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G182">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.27500837821099322</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>42.228232239999997</v>
       </c>
@@ -4178,8 +4909,12 @@
       <c r="F183" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G183">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.30641387572904027</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>42.969404930000003</v>
       </c>
@@ -4198,8 +4933,12 @@
       <c r="F184" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G184">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.28946331426518823</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>35.309102799999998</v>
       </c>
@@ -4218,8 +4957,12 @@
       <c r="F185" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G185">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.28140968430341462</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>39.5734742</v>
       </c>
@@ -4238,8 +4981,12 @@
       <c r="F186" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G186">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.27917677743554242</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>35.911303799999999</v>
       </c>
@@ -4258,8 +5005,12 @@
       <c r="F187" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G187">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.29091551584263237</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>41.833650740000003</v>
       </c>
@@ -4278,8 +5029,12 @@
       <c r="F188" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G188">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.31464463249336994</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>39.837383459999998</v>
       </c>
@@ -4298,8 +5053,12 @@
       <c r="F189" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G189">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.2902960755806791</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>43.959261750000003</v>
       </c>
@@ -4318,8 +5077,12 @@
       <c r="F190" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G190">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.25590899454839022</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>43.865276540000004</v>
       </c>
@@ -4338,8 +5101,12 @@
       <c r="F191" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G191">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.25070152800786438</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>28.19558413</v>
       </c>
@@ -4358,8 +5125,12 @@
       <c r="F192" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G192">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.25605649569782191</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>30.397043440000001</v>
       </c>
@@ -4378,8 +5149,12 @@
       <c r="F193" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G193">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.26997390315209646</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>31.61541394</v>
       </c>
@@ -4398,8 +5173,12 @@
       <c r="F194" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G194">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.29445852727583544</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>32.498443610000002</v>
       </c>
@@ -4418,8 +5197,12 @@
       <c r="F195" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G195">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.27366677749887941</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>35.083772209999999</v>
       </c>
@@ -4438,8 +5221,12 @@
       <c r="F196" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G196">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.28317053247869378</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>33.380995550000002</v>
       </c>
@@ -4458,8 +5245,12 @@
       <c r="F197" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G197">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.29677667354345338</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>30.446362480000001</v>
       </c>
@@ -4478,8 +5269,12 @@
       <c r="F198" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G198">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.25824450508657498</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>30.621447119999999</v>
       </c>
@@ -4498,8 +5293,12 @@
       <c r="F199" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G199">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.28449814988781852</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>30.59811294</v>
       </c>
@@ -4518,8 +5317,12 @@
       <c r="F200" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G200">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.28373365941991679</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>28.147852910000001</v>
       </c>
@@ -4538,8 +5341,12 @@
       <c r="F201" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G201">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.30999272235749464</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>25.92552263</v>
       </c>
@@ -4558,8 +5365,12 @@
       <c r="F202" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G202">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.26163339207351322</v>
+      </c>
+    </row>
+    <row r="203" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>26.611298009999999</v>
       </c>
@@ -4578,8 +5389,12 @@
       <c r="F203" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G203">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.26742634008586064</v>
+      </c>
+    </row>
+    <row r="204" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>43.182471640000003</v>
       </c>
@@ -4598,8 +5413,12 @@
       <c r="F204" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G204">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.27783943502805042</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>44.25974093</v>
       </c>
@@ -4618,8 +5437,12 @@
       <c r="F205" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G205">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.28420138552800628</v>
+      </c>
+    </row>
+    <row r="206" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A206">
         <v>34.317974589999999</v>
       </c>
@@ -4638,8 +5461,12 @@
       <c r="F206" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G206">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.29733437937328594</v>
+      </c>
+    </row>
+    <row r="207" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A207">
         <v>44.356719689999998</v>
       </c>
@@ -4658,8 +5485,12 @@
       <c r="F207" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G207">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.26640353042253162</v>
+      </c>
+    </row>
+    <row r="208" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A208">
         <v>45.018792789999999</v>
       </c>
@@ -4678,8 +5509,12 @@
       <c r="F208" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G208">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.29702450546647025</v>
+      </c>
+    </row>
+    <row r="209" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A209">
         <v>36.873169390000001</v>
       </c>
@@ -4698,8 +5533,12 @@
       <c r="F209" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G209">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.26924802828660804</v>
+      </c>
+    </row>
+    <row r="210" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A210">
         <v>28.288668919999999</v>
       </c>
@@ -4718,8 +5557,12 @@
       <c r="F210" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G210">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.26590283384470353</v>
+      </c>
+    </row>
+    <row r="211" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A211">
         <v>21.29434238</v>
       </c>
@@ -4738,8 +5581,12 @@
       <c r="F211" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G211">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.26097828100560039</v>
+      </c>
+    </row>
+    <row r="212" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A212">
         <v>47.059691630000003</v>
       </c>
@@ -4758,8 +5605,12 @@
       <c r="F212" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G212">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.28848819557878502</v>
+      </c>
+    </row>
+    <row r="213" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A213">
         <v>34.519972060000001</v>
       </c>
@@ -4778,8 +5629,12 @@
       <c r="F213" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G213">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.25463150583443095</v>
+      </c>
+    </row>
+    <row r="214" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A214">
         <v>27.92045401</v>
       </c>
@@ -4798,8 +5653,12 @@
       <c r="F214" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G214">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.25741207952424006</v>
+      </c>
+    </row>
+    <row r="215" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A215">
         <v>24.723408240000001</v>
       </c>
@@ -4818,8 +5677,12 @@
       <c r="F215" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G215">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.2696203328252722</v>
+      </c>
+    </row>
+    <row r="216" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A216">
         <v>33.435992149999997</v>
       </c>
@@ -4838,8 +5701,12 @@
       <c r="F216" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G216">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.29927816722437001</v>
+      </c>
+    </row>
+    <row r="217" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A217">
         <v>22.633849529999999</v>
       </c>
@@ -4858,8 +5725,12 @@
       <c r="F217" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G217">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.27747026382356388</v>
+      </c>
+    </row>
+    <row r="218" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A218">
         <v>28.752204389999999</v>
       </c>
@@ -4878,8 +5749,12 @@
       <c r="F218" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G218">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.27921719473531331</v>
+      </c>
+    </row>
+    <row r="219" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A219">
         <v>22.08744351</v>
       </c>
@@ -4897,6 +5772,10 @@
       </c>
       <c r="F219" s="1" t="s">
         <v>22</v>
+      </c>
+      <c r="G219">
+        <f>Ratio_Identifiers_Update[[#This Row],[PecFinLengths]]/Ratio_Identifiers_Update[[#This Row],[fishStdLength]]</f>
+        <v>0.25724111937393196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>